<commit_message>
Added events to calibration figures
</commit_message>
<xml_diff>
--- a/Development/Results/hypopara.model.xlsx
+++ b/Development/Results/hypopara.model.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
   <si>
     <t xml:space="preserve">names</t>
   </si>
@@ -44,18 +44,6 @@
     <t xml:space="preserve">calibrated.readmission</t>
   </si>
   <si>
-    <t xml:space="preserve">OR.simple</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI.simple</t>
-  </si>
-  <si>
-    <t xml:space="preserve">shrunk.OR.simple</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chi.simple</t>
-  </si>
-  <si>
     <t xml:space="preserve">Intercept</t>
   </si>
   <si>
@@ -83,12 +71,6 @@
     <t xml:space="preserve">0.69</t>
   </si>
   <si>
-    <t xml:space="preserve">0.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.00; 0.00]</t>
-  </si>
-  <si>
     <t xml:space="preserve">dPTH</t>
   </si>
   <si>
@@ -113,15 +95,6 @@
     <t xml:space="preserve">1.06</t>
   </si>
   <si>
-    <t xml:space="preserve">1.10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[1.06; 1.14]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">28.3</t>
-  </si>
-  <si>
     <t xml:space="preserve">CorrCa24u</t>
   </si>
   <si>
@@ -245,10 +218,7 @@
     <t xml:space="preserve">[0.84; 0.92]</t>
   </si>
   <si>
-    <t xml:space="preserve">0.85</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.81; 0.90]</t>
+    <t xml:space="preserve">0.86 [0.84; 0.92]</t>
   </si>
 </sst>
 </file>
@@ -611,413 +581,293 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
         <v>15</v>
       </c>
-      <c r="C2" t="s">
+      <c r="G2" t="s">
         <v>16</v>
       </c>
-      <c r="D2" t="s">
+      <c r="H2" t="s">
         <v>17</v>
       </c>
-      <c r="E2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" t="s">
-        <v>21</v>
-      </c>
       <c r="I2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="J2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L2" t="s">
-        <v>24</v>
-      </c>
-      <c r="M2" t="s">
-        <v>23</v>
-      </c>
-      <c r="N2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" t="s">
         <v>25</v>
       </c>
-      <c r="B3" t="s">
+      <c r="J3" t="s">
         <v>26</v>
-      </c>
-      <c r="C3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3" t="s">
-        <v>30</v>
-      </c>
-      <c r="H3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I3" t="s">
-        <v>31</v>
-      </c>
-      <c r="J3" t="s">
-        <v>32</v>
-      </c>
-      <c r="K3" t="s">
-        <v>33</v>
-      </c>
-      <c r="L3" t="s">
-        <v>34</v>
-      </c>
-      <c r="M3" t="s">
-        <v>26</v>
-      </c>
-      <c r="N3" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" t="s">
         <v>36</v>
-      </c>
-      <c r="B4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E4" t="s">
-        <v>40</v>
-      </c>
-      <c r="F4" t="s">
-        <v>41</v>
-      </c>
-      <c r="G4" t="s">
-        <v>42</v>
-      </c>
-      <c r="H4" t="s">
-        <v>43</v>
-      </c>
-      <c r="I4" t="s">
-        <v>44</v>
-      </c>
-      <c r="J4" t="s">
-        <v>45</v>
-      </c>
-      <c r="K4" t="s">
-        <v>18</v>
-      </c>
-      <c r="L4" t="s">
-        <v>18</v>
-      </c>
-      <c r="M4" t="s">
-        <v>18</v>
-      </c>
-      <c r="N4" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I5" t="s">
+        <v>45</v>
+      </c>
+      <c r="J5" t="s">
         <v>46</v>
-      </c>
-      <c r="B5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D5" t="s">
-        <v>49</v>
-      </c>
-      <c r="E5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F5" t="s">
-        <v>51</v>
-      </c>
-      <c r="G5" t="s">
-        <v>52</v>
-      </c>
-      <c r="H5" t="s">
-        <v>53</v>
-      </c>
-      <c r="I5" t="s">
-        <v>54</v>
-      </c>
-      <c r="J5" t="s">
-        <v>55</v>
-      </c>
-      <c r="K5" t="s">
-        <v>18</v>
-      </c>
-      <c r="L5" t="s">
-        <v>18</v>
-      </c>
-      <c r="M5" t="s">
-        <v>18</v>
-      </c>
-      <c r="N5" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="B6" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C6" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D6" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="E6" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="F6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="H6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="I6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="J6" t="s">
-        <v>18</v>
-      </c>
-      <c r="K6" t="s">
-        <v>18</v>
-      </c>
-      <c r="L6" t="s">
-        <v>18</v>
-      </c>
-      <c r="M6" t="s">
-        <v>18</v>
-      </c>
-      <c r="N6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B7" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="C7" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="D7" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="E7" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="F7" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G7" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="H7" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="I7" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="J7" t="s">
-        <v>18</v>
-      </c>
-      <c r="K7" t="s">
-        <v>18</v>
-      </c>
-      <c r="L7" t="s">
-        <v>18</v>
-      </c>
-      <c r="M7" t="s">
-        <v>18</v>
-      </c>
-      <c r="N7" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="D8" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="E8" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="F8" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G8" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="H8" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="I8" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="J8" t="s">
-        <v>18</v>
-      </c>
-      <c r="K8" t="s">
-        <v>18</v>
-      </c>
-      <c r="L8" t="s">
-        <v>18</v>
-      </c>
-      <c r="M8" t="s">
-        <v>18</v>
-      </c>
-      <c r="N8" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="B9" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="C9" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="D9" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="E9" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="F9" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G9" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="H9" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="I9" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="J9" t="s">
-        <v>18</v>
-      </c>
-      <c r="K9" t="s">
-        <v>18</v>
-      </c>
-      <c r="L9" t="s">
-        <v>18</v>
-      </c>
-      <c r="M9" t="s">
-        <v>18</v>
-      </c>
-      <c r="N9" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B10" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C10" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="D10" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E10" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F10" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="G10" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="H10" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="I10" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="J10" t="s">
-        <v>18</v>
-      </c>
-      <c r="K10" t="s">
-        <v>77</v>
-      </c>
-      <c r="L10" t="s">
-        <v>78</v>
-      </c>
-      <c r="M10" t="s">
-        <v>18</v>
-      </c>
-      <c r="N10" t="s">
-        <v>18</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>